<commit_message>
Add custom waveform in Verilog
</commit_message>
<xml_diff>
--- a/wire protocol.xlsx
+++ b/wire protocol.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangqr\Files\src\osc1lite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoonGroup\Documents\wangqr\osc1lite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27281520-175A-4E0B-A883-FA0DEADA367C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{3C1316E9-FD21-48AD-9446-B65CC090DA01}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>0x00</t>
   </si>
@@ -312,7 +311,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,7 +469,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -486,25 +485,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -516,10 +507,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -836,11 +850,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F55FEF-398F-482E-9085-D00C0638D701}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,344 +922,344 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
       <c r="J8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="18"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="13" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -1268,10 +1282,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
@@ -1291,10 +1305,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="6" t="s">
         <v>32</v>
       </c>
@@ -1388,19 +1402,19 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="18"/>
       <c r="D28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="13"/>
       <c r="D29" t="s">
         <v>76</v>
       </c>
@@ -1465,73 +1479,73 @@
       <c r="B33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
@@ -1617,76 +1631,76 @@
       <c r="A44" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
@@ -1772,48 +1786,48 @@
       <c r="A55" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
-      <c r="N55" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
       <c r="Q56" s="8" t="s">
         <v>11</v>
       </c>
@@ -1822,23 +1836,23 @@
       <c r="A57" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="9"/>
-      <c r="P57" s="9"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
       <c r="Q57" s="8" t="s">
         <v>11</v>
       </c>
@@ -1847,23 +1861,23 @@
       <c r="A58" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
-      <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
-      <c r="O58" s="9"/>
-      <c r="P58" s="9"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
       <c r="Q58" s="8" t="s">
         <v>11</v>
       </c>
@@ -1872,23 +1886,23 @@
       <c r="A59" t="s">
         <v>67</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
       <c r="Q59" s="8" t="s">
         <v>11</v>
       </c>
@@ -2065,136 +2079,146 @@
       </c>
     </row>
     <row r="67" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="9" t="s">
+      <c r="C67" s="23"/>
+      <c r="D67" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="16"/>
     </row>
     <row r="68" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+      <c r="L68" s="22"/>
+      <c r="M68" s="22"/>
+      <c r="N68" s="22"/>
+      <c r="O68" s="22"/>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="16"/>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="9"/>
-      <c r="O70" s="9"/>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="9"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="16"/>
     </row>
     <row r="71" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
-      <c r="O71" s="9"/>
-      <c r="P71" s="9"/>
-      <c r="Q71" s="9"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="16"/>
     </row>
     <row r="72" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="23"/>
+      <c r="K72" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="16"/>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C74" s="20"/>
+      <c r="C74" s="9"/>
       <c r="D74" t="s">
         <v>88</v>
       </c>
@@ -2218,34 +2242,40 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B70:Q70"/>
-    <mergeCell ref="B71:Q71"/>
-    <mergeCell ref="B72:Q72"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="J67:M67"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="N67:Q67"/>
-    <mergeCell ref="B68:Q68"/>
-    <mergeCell ref="B69:Q69"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="C33:Q33"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="E3:Q3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="B9:Q9"/>
-    <mergeCell ref="B10:M10"/>
+  <mergeCells count="72">
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="B69:J69"/>
+    <mergeCell ref="K69:Q69"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="B71:J71"/>
+    <mergeCell ref="K70:Q70"/>
+    <mergeCell ref="K71:Q71"/>
+    <mergeCell ref="B59:P59"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B55:M55"/>
+    <mergeCell ref="N55:Q55"/>
+    <mergeCell ref="B56:P56"/>
+    <mergeCell ref="B57:P57"/>
+    <mergeCell ref="B58:P58"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B44:M44"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B4:Q4"/>
@@ -2262,31 +2292,29 @@
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="J12:M12"/>
     <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="B45:M45"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="N44:Q44"/>
-    <mergeCell ref="N45:Q45"/>
-    <mergeCell ref="N46:Q46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B59:P59"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B55:M55"/>
-    <mergeCell ref="N55:Q55"/>
-    <mergeCell ref="B56:P56"/>
-    <mergeCell ref="B57:P57"/>
-    <mergeCell ref="B58:P58"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C33:Q33"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B68:P68"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="J67:N67"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:I67"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B72:J72"/>
+    <mergeCell ref="K72:Q72"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>